<commit_message>
Amélioration de la fonction de recherche de produits en remplaçant le champ de texte par une liste déroulante de produits uniques. Mise à jour de la logique de filtrage pour sélectionner un produit spécifique. Modifications des fichiers Excel 'emplacements.xlsx' et 'fournisseurs.xlsx' pour refléter les changements récents.
</commit_message>
<xml_diff>
--- a/data/emplacements.xlsx
+++ b/data/emplacements.xlsx
@@ -637,10 +637,10 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>